<commit_message>
reception and administrator section was modified
</commit_message>
<xml_diff>
--- a/datos_albergue.xlsx
+++ b/datos_albergue.xlsx
@@ -517,68 +517,78 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>folio</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>nombre</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>identificacion</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>edad</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>fecha_nacimiento</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>nacionalidad</t>
         </is>
       </c>
-      <c r="G1" s="3" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>genero</t>
         </is>
       </c>
-      <c r="H1" s="3" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>tipo</t>
         </is>
       </c>
-      <c r="I1" s="3" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>tutor_folio</t>
         </is>
       </c>
-      <c r="J1" s="3" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>fecha_ingreso</t>
         </is>
       </c>
-      <c r="K1" s="3" t="inlineStr">
+      <c r="K1" s="4" t="inlineStr">
         <is>
           <t>num_acompanantes</t>
+        </is>
+      </c>
+      <c r="L1" s="4" t="inlineStr">
+        <is>
+          <t>fecha_salida</t>
+        </is>
+      </c>
+      <c r="M1" s="4" t="inlineStr">
+        <is>
+          <t>motivo_salida</t>
         </is>
       </c>
     </row>
@@ -592,7 +602,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1312312312</v>
+        <v>13123123128</v>
       </c>
       <c r="D2" t="n">
         <v>25</v>
@@ -617,13 +627,24 @@
           <t>Titular</t>
         </is>
       </c>
+      <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
           <t>2025-12-12</t>
         </is>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>2025-12-17 12:29:16</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>trabajo</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -673,6 +694,77 @@
       </c>
       <c r="K3" t="n">
         <v>0</v>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>2025-12-17 12:29:16</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>trabajo</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1001-B</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Luna Ochoa D L</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>s123s123s12</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2025-04-10</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Americana</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Femenino</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Acompañante</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>1001</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>2025-12-17</t>
+        </is>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>2025-12-17 12:29:16</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>trabajo</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -787,8 +879,6 @@
           <t>casa</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">

</xml_diff>

<commit_message>
added module enfermeria and fixed admin
</commit_message>
<xml_diff>
--- a/datos_albergue.xlsx
+++ b/datos_albergue.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -766,6 +766,57 @@
           <t>trabajo</t>
         </is>
       </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1002</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>juan perez</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>8sdausd8a0sd8j</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>27</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1998-01-14</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>americana</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Titular</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>2025-12-17 13:27:20</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>